<commit_message>
Add images and excerpts from Strasbourg catalogue.
</commit_message>
<xml_diff>
--- a/info/general.xlsx
+++ b/info/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\dev\home\paveloom\Repositories\Packs\P11\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96450E27-B0AB-44FF-B688-174723823669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDC0D27-4CC4-4B2A-8DC8-9CBBECB43C13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="168" windowWidth="23040" windowHeight="12792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10740" yWindow="1392" windowWidth="23040" windowHeight="12792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>[Ca V]</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Hα</t>
-  </si>
-  <si>
-    <t>[O III], Hα</t>
   </si>
 </sst>
 </file>
@@ -231,9 +228,24 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -241,21 +253,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -541,7 +538,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,187 +552,187 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.8" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="A3" s="1">
         <v>6087</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="1">
         <v>7005</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="7" t="s">
+      <c r="D4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="A5" s="1">
         <v>6434</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="A6" s="1">
         <v>6101</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="1">
         <v>7531</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="7" t="s">
+      <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="1">
         <v>8046</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="1">
         <v>4686</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="7" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="7" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>20</v>
+      <c r="F10" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the pictures, tutorial and report.
</commit_message>
<xml_diff>
--- a/info/general.xlsx
+++ b/info/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\dev\home\paveloom\Repositories\Packs\P11\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDC0D27-4CC4-4B2A-8DC8-9CBBECB43C13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B13EF72-026E-47B7-AE83-C32E38681BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10740" yWindow="1392" windowWidth="23040" windowHeight="12792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="168" windowWidth="23040" windowHeight="12792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -538,7 +538,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F10" sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>